<commit_message>
Fixed up inconsistencies in sprint 2
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint2/execution.xlsx
+++ b/sprint_backlog/sprint2/execution.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajg\Documents\Repositories\CSCC01\Team5\sprint_backlog\sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A63891-1C9B-4496-B6AF-FE437E254F6A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AE38A8-D2A8-46D3-8290-472382233992}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13963" windowHeight="5263" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="5265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <r>
       <rPr>
@@ -182,9 +182,6 @@
     <t>Changes in Story Points</t>
   </si>
   <si>
-    <t>Alex ran into an unexpected problem with Excel sheet part of T7 (ended up needing to write a VBA script) and as a result was unable to finish T7 completely. He estimates that he needs an extra 1 story point next sprint to finish it.</t>
-  </si>
-  <si>
     <t>A:2</t>
   </si>
   <si>
@@ -203,7 +200,16 @@
     <t>W:2</t>
   </si>
   <si>
-    <t>Won was unable to finish T5 on time due to other academic obligations and estimates that he needs 1 more story point next sprint to complete it.</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Alex ran into an unexpected problem with Excel sheet part of T7 (ended up needing to write a VBA script) and as a result was unable to finish T7 completely. He estimates that he needs 2 extra story points next sprint to finish it.</t>
+  </si>
+  <si>
+    <t>Won was unable to finish T5 on time due to other academic obligations and estimates that he also needs 2 more story points next sprint to complete it.</t>
   </si>
 </sst>
 </file>
@@ -284,19 +290,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -315,29 +308,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,35 +735,37 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" activeCellId="1" sqref="A21:I22 D26"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.3046875" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" customWidth="1"/>
-    <col min="3" max="3" width="16.53515625" customWidth="1"/>
-    <col min="4" max="4" width="11.53515625" customWidth="1"/>
-    <col min="5" max="1025" width="8.3046875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="9" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7"/>
@@ -766,8 +776,9 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -795,8 +806,11 @@
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -810,16 +824,19 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -833,20 +850,21 @@
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>46</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -874,9 +892,12 @@
       <c r="I6" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="8" t="s">
+      <c r="J6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -888,20 +909,21 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -915,14 +937,17 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -939,9 +964,10 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A10" s="8"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
@@ -956,8 +982,9 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -975,8 +1002,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -994,8 +1022,9 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1013,8 +1042,9 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1032,88 +1062,95 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="9" t="s">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A18:I20"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A21:J22"/>
+    <mergeCell ref="A17:J17"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A18:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>